<commit_message>
I hope  it is final  changing
</commit_message>
<xml_diff>
--- a/src/test/resources/Тест-кейсы.xlsx
+++ b/src/test/resources/Тест-кейсы.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Тест кейсы</t>
   </si>
@@ -98,6 +98,38 @@
   <si>
     <t>Клиенты были отсортированы  в 
 обратном порядке</t>
+  </si>
+  <si>
+    <t>Создание пользователя с пустыми параметрами</t>
+  </si>
+  <si>
+    <t>1)Нажать на кнопку 'Add customer'
+2)Заполнить поле FirstName значением ' '
+3)Заполнить поле LastName значением ' '
+4)Заполнить поле PostalCode значением ' '
+5)Нажать на кнопку 'Add customer'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Появится alert-окно с надписью
+ 'Please check the details. Customer may be duplicate'
+</t>
+  </si>
+  <si>
+    <t>комментарии</t>
+  </si>
+  <si>
+    <t>P.S: про поиске данный пользователь не был найден</t>
+  </si>
+  <si>
+    <t>1)Нажать на кнопку 'Add customer'
+2)Внизу нажать на кнопку 'Add customer'</t>
+  </si>
+  <si>
+    <t>Не появится alert-окно с надписью
+ 'Customer added successfully with customer id :...'</t>
+  </si>
+  <si>
+    <t>Негативный сценарий:пользователь не создан</t>
   </si>
 </sst>
 </file>
@@ -134,7 +166,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -144,9 +176,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,9 +490,10 @@
     <col min="2" max="2" width="81" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="31.88671875" customWidth="1"/>
+    <col min="5" max="5" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,8 +506,11 @@
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="130.19999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -491,7 +524,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -505,7 +538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="126" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="126" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -519,7 +552,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -533,7 +566,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -547,9 +580,36 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
+    <row r="7" spans="1:5" ht="117.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>